<commit_message>
Menu updates for documentation
</commit_message>
<xml_diff>
--- a/Doc/V2X Project Scope.xlsx
+++ b/Doc/V2X Project Scope.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesse\Documents\JopelDesigns\Projects\rvi_v2x_firmware\Doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="96" yWindow="72" windowWidth="11460" windowHeight="5568"/>
+    <workbookView xWindow="96" yWindow="672" windowWidth="11460" windowHeight="5568"/>
   </bookViews>
   <sheets>
     <sheet name="V2X project definition" sheetId="1" r:id="rId1"/>
@@ -15,12 +20,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'V2X project definition'!$A$1:$E$59</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="112">
   <si>
     <t>GPS</t>
   </si>
@@ -340,9 +344,6 @@
     <t>GPS samples are compared to determin motion trigger</t>
   </si>
   <si>
-    <t>The GPS system can be started and stopped by AT cmd on SIM USB</t>
-  </si>
-  <si>
     <t>Serial controller</t>
   </si>
   <si>
@@ -356,6 +357,9 @@
   </si>
   <si>
     <t>enable/disable watchdog service while HOST is asleep</t>
+  </si>
+  <si>
+    <t>The GPS system can be started and stopped by AT cmd or SIM USB</t>
   </si>
 </sst>
 </file>
@@ -402,6 +406,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -450,7 +457,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -485,7 +492,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -696,9 +703,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:E59"/>
+      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -952,6 +959,9 @@
       <c r="D15" t="s">
         <v>102</v>
       </c>
+      <c r="E15" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -966,6 +976,9 @@
       <c r="D16" t="s">
         <v>103</v>
       </c>
+      <c r="E16" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -978,7 +991,10 @@
         <v>88</v>
       </c>
       <c r="D17" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+      <c r="E17" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -989,13 +1005,13 @@
         <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1042,6 +1058,9 @@
       <c r="D21" t="s">
         <v>28</v>
       </c>
+      <c r="E21" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -1056,6 +1075,9 @@
       <c r="D22" t="s">
         <v>20</v>
       </c>
+      <c r="E22" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -1069,6 +1091,9 @@
       </c>
       <c r="D23" t="s">
         <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1112,6 +1137,9 @@
       <c r="D26" t="s">
         <v>54</v>
       </c>
+      <c r="E26" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -1121,10 +1149,10 @@
         <v>46</v>
       </c>
       <c r="C27" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" t="s">
         <v>110</v>
-      </c>
-      <c r="D27" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1154,6 +1182,9 @@
       <c r="D29" t="s">
         <v>44</v>
       </c>
+      <c r="E29" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -1213,6 +1244,9 @@
       <c r="D33" t="s">
         <v>87</v>
       </c>
+      <c r="E33" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -1225,7 +1259,7 @@
         <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E34" t="s">
         <v>80</v>
@@ -1349,7 +1383,7 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D42" t="s">
         <v>73</v>
@@ -1484,6 +1518,9 @@
       <c r="D50" t="s">
         <v>63</v>
       </c>
+      <c r="E50" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
@@ -1498,6 +1535,9 @@
       <c r="D51" t="s">
         <v>75</v>
       </c>
+      <c r="E51" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
@@ -1614,6 +1654,9 @@
       <c r="D58" t="s">
         <v>17</v>
       </c>
+      <c r="E58" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
@@ -1627,6 +1670,9 @@
       </c>
       <c r="D59" t="s">
         <v>36</v>
+      </c>
+      <c r="E59" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>